<commit_message>
K Update Table Description and Definition
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-kds2db\kds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB1ECE6-DCC2-4B9C-A664-1D4CBAB02A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4AE98E-EAC3-4F26-92FA-8559FBB9B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="249">
   <si>
     <t>resource</t>
   </si>
@@ -777,6 +777,15 @@
   </si>
   <si>
     <t>referenceRange/type/CodeableConcept</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>ward_name</t>
   </si>
 </sst>
 </file>
@@ -1232,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C155" sqref="C155"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2927,6 +2936,9 @@
       <c r="A232" t="s">
         <v>154</v>
       </c>
+      <c r="C232" t="s">
+        <v>246</v>
+      </c>
       <c r="D232" t="s">
         <v>155</v>
       </c>
@@ -2935,6 +2947,9 @@
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C233" t="s">
+        <v>248</v>
+      </c>
       <c r="D233" t="s">
         <v>156</v>
       </c>
@@ -2943,6 +2958,9 @@
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C234" t="s">
+        <v>247</v>
+      </c>
       <c r="D234" t="s">
         <v>156</v>
       </c>
@@ -3046,7 +3064,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
K + DB Recreate TableDescription and SQL Statements
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-kds2db\kds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4AE98E-EAC3-4F26-92FA-8559FBB9B89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B87FC1D-7872-46CC-9141-47363B8B02A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="248">
   <si>
     <t>resource</t>
   </si>
@@ -354,9 +354,6 @@
   </si>
   <si>
     <t>medstat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>dateAsserted</t>
@@ -1241,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,9 +2137,6 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>105</v>
-      </c>
       <c r="C121" s="2" t="s">
         <v>15</v>
       </c>
@@ -2231,7 +2225,7 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C133" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D133" t="s">
         <v>50</v>
@@ -2242,12 +2236,12 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C134" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C135" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -2273,7 +2267,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F139">
         <v>2</v>
@@ -2281,10 +2275,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>109</v>
+      </c>
+      <c r="B141" t="s">
         <v>110</v>
-      </c>
-      <c r="B141" t="s">
-        <v>111</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>12</v>
@@ -2361,7 +2355,7 @@
     </row>
     <row r="151" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D151" t="s">
         <v>50</v>
@@ -2372,7 +2366,7 @@
     </row>
     <row r="152" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F152">
         <v>2</v>
@@ -2380,7 +2374,7 @@
     </row>
     <row r="153" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C153" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F153">
         <v>2</v>
@@ -2388,7 +2382,7 @@
     </row>
     <row r="154" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C154" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F154">
         <v>2</v>
@@ -2396,7 +2390,7 @@
     </row>
     <row r="155" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F155">
         <v>2</v>
@@ -2404,7 +2398,7 @@
     </row>
     <row r="156" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="157" spans="3:6" x14ac:dyDescent="0.25">
@@ -2414,17 +2408,17 @@
     </row>
     <row r="158" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="159" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C159" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="160" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F160">
         <v>3</v>
@@ -2432,7 +2426,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C161" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F161">
         <v>3</v>
@@ -2440,7 +2434,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F162">
         <v>3</v>
@@ -2448,7 +2442,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F163">
         <v>3</v>
@@ -2456,7 +2450,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F164">
         <v>3</v>
@@ -2464,7 +2458,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C165" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E165">
         <v>500</v>
@@ -2472,15 +2466,15 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C166" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
+        <v>124</v>
+      </c>
+      <c r="B168" t="s">
         <v>125</v>
-      </c>
-      <c r="B168" t="s">
-        <v>126</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>12</v>
@@ -2523,7 +2517,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C173" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E173">
         <v>70</v>
@@ -2531,7 +2525,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C174" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E174">
         <v>70</v>
@@ -2571,7 +2565,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C179" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D179" t="s">
         <v>50</v>
@@ -2582,12 +2576,12 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C180" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C181" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E181">
         <v>500</v>
@@ -2595,15 +2589,15 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C182" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>130</v>
+      </c>
+      <c r="B184" t="s">
         <v>131</v>
-      </c>
-      <c r="B184" t="s">
-        <v>132</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>12</v>
@@ -2643,7 +2637,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C189" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E189">
         <v>30</v>
@@ -2677,20 +2671,20 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C194" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C195" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>134</v>
+      </c>
+      <c r="B197" t="s">
         <v>135</v>
-      </c>
-      <c r="B197" t="s">
-        <v>136</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>12</v>
@@ -2761,7 +2755,7 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D207" t="s">
         <v>50</v>
@@ -2772,7 +2766,7 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C208" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,10 +2789,10 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>138</v>
+      </c>
+      <c r="B213" t="s">
         <v>139</v>
-      </c>
-      <c r="B213" t="s">
-        <v>140</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>12</v>
@@ -2809,7 +2803,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C214" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E214">
         <v>70</v>
@@ -2833,12 +2827,12 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C217" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C218" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D218" t="s">
         <v>50</v>
@@ -2849,7 +2843,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C219" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E219">
         <v>10</v>
@@ -2857,30 +2851,30 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C220" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C221" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C222" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C223" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>148</v>
+      </c>
+      <c r="B225" t="s">
         <v>149</v>
-      </c>
-      <c r="B225" t="s">
-        <v>150</v>
       </c>
       <c r="C225" t="s">
         <v>12</v>
@@ -2907,7 +2901,7 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C228" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E228">
         <v>50</v>
@@ -2915,7 +2909,7 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C229" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E229">
         <v>50</v>
@@ -2923,7 +2917,7 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C230" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E230">
         <v>30</v>
@@ -2934,13 +2928,13 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>153</v>
+      </c>
+      <c r="C232" t="s">
+        <v>245</v>
+      </c>
+      <c r="D232" t="s">
         <v>154</v>
-      </c>
-      <c r="C232" t="s">
-        <v>246</v>
-      </c>
-      <c r="D232" t="s">
-        <v>155</v>
       </c>
       <c r="E232">
         <v>25</v>
@@ -2948,10 +2942,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C233" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D233" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E233">
         <v>30</v>
@@ -2959,10 +2953,10 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C234" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D234" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E234">
         <v>30</v>
@@ -2970,96 +2964,96 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B240" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B241" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B241" s="4" t="s">
+      <c r="D241" t="s">
         <v>164</v>
-      </c>
-      <c r="D241" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B242" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="B242" s="4" t="s">
+      <c r="D242" t="s">
         <v>167</v>
-      </c>
-      <c r="D242" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B243" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B243" s="4" t="s">
+      <c r="D243" t="s">
         <v>170</v>
-      </c>
-      <c r="D243" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B244" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B244" s="4" t="s">
+      <c r="D244" t="s">
         <v>173</v>
-      </c>
-      <c r="D244" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B245" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B245" s="4" t="s">
+      <c r="D245" t="s">
         <v>176</v>
-      </c>
-      <c r="D245" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B246" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="D246" t="s">
         <v>179</v>
-      </c>
-      <c r="D246" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3092,10 +3086,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3103,7 +3097,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3111,7 +3105,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3119,7 +3113,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3127,7 +3121,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3167,7 +3161,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3178,7 +3172,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -3186,7 +3180,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
@@ -3197,7 +3191,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -3237,12 +3231,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3279,10 +3273,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3290,7 +3284,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3298,7 +3292,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3306,7 +3300,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3314,7 +3308,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3356,7 +3350,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -3367,7 +3361,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3375,7 +3369,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3383,7 +3377,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3391,12 +3385,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
         <v>71</v>
@@ -3407,67 +3401,67 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +3500,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -3520,22 +3514,22 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -3546,7 +3540,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -3557,10 +3551,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3568,10 +3562,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -3579,7 +3573,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -3587,7 +3581,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -3598,7 +3592,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -3609,10 +3603,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -3620,10 +3614,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -3631,7 +3625,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -3639,7 +3633,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3650,10 +3644,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -3664,7 +3658,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -3675,7 +3669,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -3725,7 +3719,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3733,12 +3727,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -3746,7 +3740,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3754,7 +3748,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3791,7 +3785,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3807,7 +3801,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3815,12 +3809,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3862,7 +3856,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -3870,7 +3864,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3913,7 +3907,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3921,7 +3915,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -3929,7 +3923,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3937,7 +3931,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3973,7 +3967,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
@@ -3984,7 +3978,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
@@ -4026,10 +4020,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4037,7 +4031,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -4045,7 +4039,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4053,7 +4047,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -4061,7 +4055,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -4101,12 +4095,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4143,10 +4137,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4154,7 +4148,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -4162,7 +4156,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -4170,7 +4164,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5">
         <v>30</v>

</xml_diff>

<commit_message>
K Update TableDescriptions and DB SQL Script
</commit_message>
<xml_diff>
--- a/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
+++ b/R-kds2db/kds2db/inst/extdata/Table_Description_Definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\D\Eigene Projekte\smith\uc-phep\interpolar\R-kds2db\kds2db\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D6A141-D188-49B7-B1E3-70058DEB7D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1070BF8-E8DA-45AE-82AE-7DB60B5F20CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="621" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_description_collapsed" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,11 @@
     <sheet name="Quantity" sheetId="13" r:id="rId13"/>
     <sheet name="Dosage" sheetId="14" r:id="rId14"/>
     <sheet name="Timing" sheetId="15" r:id="rId15"/>
+    <sheet name="Datatypes" sheetId="16" r:id="rId16"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table_description_collapsed!$F$8:$G$12</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="251">
   <si>
     <t>resource</t>
   </si>
@@ -518,9 +522,6 @@
     <t>ward_name</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>patient_id</t>
   </si>
   <si>
@@ -783,13 +784,25 @@
   </si>
   <si>
     <t>repeat/offset</t>
+  </si>
+  <si>
+    <t>datatypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string </t>
+  </si>
+  <si>
+    <t>Ein leerer Wert bedeutet automatisch string</t>
+  </si>
+  <si>
+    <t>Diese Tabelle enthält die in der Spalte type auswählbaren Datentypen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -816,6 +829,13 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -851,7 +871,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -860,6 +880,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Good" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1245,9 +1266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2583,7 +2602,6 @@
       <c r="C177" t="s">
         <v>48</v>
       </c>
-      <c r="E177" s="3"/>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
     </row>
@@ -2999,121 +3017,127 @@
       <c r="C234" t="s">
         <v>158</v>
       </c>
-      <c r="E234" t="s">
-        <v>159</v>
-      </c>
       <c r="F234">
         <v>30</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C235" t="s">
-        <v>160</v>
-      </c>
-      <c r="E235" t="s">
         <v>159</v>
       </c>
       <c r="F235">
-        <v>30</v>
+        <v>70</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B241" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B242" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B242" s="5" t="s">
+      <c r="E242" t="s">
         <v>168</v>
-      </c>
-      <c r="E242" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B243" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B243" s="5" t="s">
+      <c r="E243" t="s">
         <v>171</v>
-      </c>
-      <c r="E243" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B244" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B244" s="5" t="s">
+      <c r="E244" t="s">
         <v>174</v>
-      </c>
-      <c r="E244" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B245" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B245" s="5" t="s">
+      <c r="E245" t="s">
         <v>177</v>
-      </c>
-      <c r="E245" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B246" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B246" s="5" t="s">
+      <c r="E246" t="s">
         <v>180</v>
-      </c>
-      <c r="E246" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B247" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B247" s="5" t="s">
+      <c r="E247" t="s">
         <v>183</v>
-      </c>
-      <c r="E247" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F8A53250-F326-4B90-86EA-0D130A7F9913}">
+          <x14:formula1>
+            <xm:f>Datatypes!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E235</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3141,10 +3165,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>201</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -3152,7 +3176,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3160,7 +3184,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3168,7 +3192,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3176,7 +3200,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3216,7 +3240,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3227,7 +3251,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -3235,7 +3259,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
@@ -3246,7 +3270,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -3286,12 +3310,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3328,10 +3352,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>201</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -3339,7 +3363,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -3347,7 +3371,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3355,7 +3379,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3363,7 +3387,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -3405,7 +3429,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
@@ -3416,7 +3440,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3424,7 +3448,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -3432,7 +3456,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3440,12 +3464,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
         <v>73</v>
@@ -3456,17 +3480,17 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3476,47 +3500,47 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3530,7 +3554,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,7 +3579,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
@@ -3569,22 +3593,22 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -3595,7 +3619,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -3606,10 +3630,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3617,10 +3641,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -3628,7 +3652,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -3636,7 +3660,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -3647,7 +3671,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -3658,10 +3682,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -3669,10 +3693,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -3680,7 +3704,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -3688,7 +3712,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -3699,10 +3723,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -3713,7 +3737,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -3724,7 +3748,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
@@ -3741,6 +3765,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{671D09BB-E5B9-4217-A0D2-BB413AC8772B}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3774,7 +3860,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -3782,12 +3868,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -3795,7 +3881,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -3803,7 +3889,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3840,7 +3926,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3856,7 +3942,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3864,12 +3950,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -3911,7 +3997,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -3919,7 +4005,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3">
         <v>500</v>
@@ -3962,7 +4048,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -3970,7 +4056,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -3978,7 +4064,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -3986,7 +4072,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -4022,7 +4108,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
@@ -4033,7 +4119,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
@@ -4075,10 +4161,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>201</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4086,7 +4172,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -4094,7 +4180,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -4102,7 +4188,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C5">
         <v>70</v>
@@ -4110,7 +4196,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -4150,12 +4236,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4192,10 +4278,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
         <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>201</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -4203,7 +4289,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -4211,7 +4297,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C4">
         <v>70</v>
@@ -4219,7 +4305,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C5">
         <v>30</v>

</xml_diff>